<commit_message>
update excel sheet header
</commit_message>
<xml_diff>
--- a/server/survey_data.xlsx
+++ b/server/survey_data.xlsx
@@ -397,116 +397,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:BM2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Name</v>
+        <v>Personal Information</v>
       </c>
       <c r="B1" t="str">
-        <v>Phone</v>
+        <v/>
       </c>
       <c r="C1" t="str">
-        <v>Bike Type</v>
+        <v/>
       </c>
       <c r="D1" t="str">
         <v>Rankings</v>
       </c>
       <c r="E1" t="str">
+        <v/>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
+      <c r="H1" t="str">
+        <v/>
+      </c>
+      <c r="I1" t="str">
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <v/>
+      </c>
+      <c r="K1" t="str">
+        <v/>
+      </c>
+      <c r="L1" t="str">
+        <v/>
+      </c>
+      <c r="M1" t="str">
+        <v/>
+      </c>
+      <c r="N1" t="str">
+        <v/>
+      </c>
+      <c r="O1" t="str">
+        <v/>
+      </c>
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1" t="str">
+        <v/>
+      </c>
+      <c r="R1" t="str">
+        <v/>
+      </c>
+      <c r="S1" t="str">
+        <v/>
+      </c>
+      <c r="T1" t="str">
         <v>Product Features</v>
+      </c>
+      <c r="U1" t="str">
+        <v/>
+      </c>
+      <c r="V1" t="str">
+        <v/>
+      </c>
+      <c r="W1" t="str">
+        <v/>
+      </c>
+      <c r="X1" t="str">
+        <v/>
+      </c>
+      <c r="Y1" t="str">
+        <v/>
+      </c>
+      <c r="Z1" t="str">
+        <v/>
+      </c>
+      <c r="AA1" t="str">
+        <v/>
+      </c>
+      <c r="AB1" t="str">
+        <v/>
+      </c>
+      <c r="AC1" t="str">
+        <v/>
+      </c>
+      <c r="AD1" t="str">
+        <v/>
+      </c>
+      <c r="AE1" t="str">
+        <v/>
+      </c>
+      <c r="AF1" t="str">
+        <v/>
+      </c>
+      <c r="AG1" t="str">
+        <v/>
+      </c>
+      <c r="AH1" t="str">
+        <v/>
+      </c>
+      <c r="AI1" t="str">
+        <v/>
+      </c>
+      <c r="AJ1" t="str">
+        <v/>
+      </c>
+      <c r="AK1" t="str">
+        <v/>
+      </c>
+      <c r="AL1" t="str">
+        <v/>
+      </c>
+      <c r="AM1" t="str">
+        <v/>
+      </c>
+      <c r="AN1" t="str">
+        <v/>
+      </c>
+      <c r="AO1" t="str">
+        <v/>
+      </c>
+      <c r="AP1" t="str">
+        <v/>
+      </c>
+      <c r="AQ1" t="str">
+        <v/>
+      </c>
+      <c r="AR1" t="str">
+        <v/>
+      </c>
+      <c r="AS1" t="str">
+        <v/>
+      </c>
+      <c r="AT1" t="str">
+        <v/>
+      </c>
+      <c r="AU1" t="str">
+        <v/>
+      </c>
+      <c r="AV1" t="str">
+        <v/>
+      </c>
+      <c r="AW1" t="str">
+        <v/>
+      </c>
+      <c r="AX1" t="str">
+        <v/>
+      </c>
+      <c r="AY1" t="str">
+        <v/>
+      </c>
+      <c r="AZ1" t="str">
+        <v/>
+      </c>
+      <c r="BA1" t="str">
+        <v/>
+      </c>
+      <c r="BB1" t="str">
+        <v/>
+      </c>
+      <c r="BC1" t="str">
+        <v/>
+      </c>
+      <c r="BD1" t="str">
+        <v/>
+      </c>
+      <c r="BE1" t="str">
+        <v/>
+      </c>
+      <c r="BF1" t="str">
+        <v/>
+      </c>
+      <c r="BG1" t="str">
+        <v/>
+      </c>
+      <c r="BH1" t="str">
+        <v/>
+      </c>
+      <c r="BI1" t="str">
+        <v/>
+      </c>
+      <c r="BJ1" t="str">
+        <v/>
+      </c>
+      <c r="BK1" t="str">
+        <v/>
+      </c>
+      <c r="BL1" t="str">
+        <v/>
+      </c>
+      <c r="BM1" t="str">
+        <v/>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Jawwad Al Sabbir</v>
+        <v>Name</v>
       </c>
       <c r="B2" t="str">
-        <v>01821419398</v>
+        <v>Phone</v>
       </c>
       <c r="C2" t="str">
-        <v>asdf</v>
+        <v>Bike Type</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">, , , , , , , , , , , , , , </v>
+        <v>Row 1</v>
       </c>
       <c r="E2" t="str">
-        <v xml:space="preserve">, ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , , </v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>MD. ABDUR RAHIM SANA</v>
-      </c>
-      <c r="B3" t="str">
-        <v>01821419398</v>
-      </c>
-      <c r="C3" t="str">
-        <v>asdffjdklsj</v>
-      </c>
-      <c r="D3" t="str">
-        <v xml:space="preserve">, , , , , , , , , , , , , , </v>
-      </c>
-      <c r="E3" t="str">
-        <v xml:space="preserve">, ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , , </v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>MD. ABDUR RAHIM SANA</v>
-      </c>
-      <c r="B4" t="str">
-        <v>01821419398</v>
-      </c>
-      <c r="C4" t="str">
-        <v>asdffjdklsj</v>
-      </c>
-      <c r="D4" t="str">
-        <v xml:space="preserve">, , , , , , , , , , , , , , </v>
-      </c>
-      <c r="E4" t="str">
-        <v xml:space="preserve">, ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , , </v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Tazim</v>
-      </c>
-      <c r="B5" t="str">
-        <v>10903434</v>
-      </c>
-      <c r="C5" t="str">
-        <v>sfsfs</v>
-      </c>
-      <c r="D5" t="str">
-        <v xml:space="preserve">, , , , , , , , , , , , , , </v>
-      </c>
-      <c r="E5" t="str">
-        <v xml:space="preserve">, ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , , </v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Tanvir</v>
-      </c>
-      <c r="B6" t="str">
-        <v>017437843</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Dhaka</v>
-      </c>
-      <c r="D6" t="str">
-        <v xml:space="preserve">, , , , , , , , , , , , , , </v>
-      </c>
-      <c r="E6" t="str">
-        <v xml:space="preserve">, ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , ,  | , , </v>
+        <v>Row 2</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Row 3</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Row 4</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Row 5</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Row 6</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Row 7</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Row 8</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Row 9</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Row 10</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Row 11</v>
+      </c>
+      <c r="O2" t="str">
+        <v>Row 12</v>
+      </c>
+      <c r="P2" t="str">
+        <v>Row 13</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>Row 14</v>
+      </c>
+      <c r="R2" t="str">
+        <v>Row 15</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BM2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update for excel sheet
</commit_message>
<xml_diff>
--- a/server/survey_data.xlsx
+++ b/server/survey_data.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BM3"/>
+  <dimension ref="A1:BN3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -458,10 +458,10 @@
         <v/>
       </c>
       <c r="S1" t="str">
-        <v/>
+        <v>Product Features</v>
       </c>
       <c r="T1" t="str">
-        <v>Product Features</v>
+        <v/>
       </c>
       <c r="U1" t="str">
         <v/>
@@ -593,9 +593,12 @@
         <v/>
       </c>
       <c r="BL1" t="str">
-        <v/>
+        <v>Survey Data</v>
       </c>
       <c r="BM1" t="str">
+        <v/>
+      </c>
+      <c r="BN1" t="str">
         <v/>
       </c>
     </row>
@@ -654,6 +657,147 @@
       <c r="R2" t="str">
         <v>Row 15</v>
       </c>
+      <c r="S2" t="str">
+        <v>Speed Importance Level</v>
+      </c>
+      <c r="T2" t="str">
+        <v>Speed Satisfaction Level</v>
+      </c>
+      <c r="U2" t="str">
+        <v>Speed Fulfillment Capacity</v>
+      </c>
+      <c r="V2" t="str">
+        <v>Charging time Importance Level</v>
+      </c>
+      <c r="W2" t="str">
+        <v>Charging time Satisfaction Level</v>
+      </c>
+      <c r="X2" t="str">
+        <v>Charging time Fulfillment Capacity</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>Eco-Friendly Importance Level</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>Eco-Friendly Satisfaction Level</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>Eco-Friendly Fulfillment Capacity</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>Mileage Importance Level</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>Mileage Satisfaction Level</v>
+      </c>
+      <c r="AD2" t="str">
+        <v>Mileage Fulfillment Capacity</v>
+      </c>
+      <c r="AE2" t="str">
+        <v>Seat capacity Importance Level</v>
+      </c>
+      <c r="AF2" t="str">
+        <v>Seat capacity Satisfaction Level</v>
+      </c>
+      <c r="AG2" t="str">
+        <v>Seat capacity Fulfillment Capacity</v>
+      </c>
+      <c r="AH2" t="str">
+        <v>Brand Importance Level</v>
+      </c>
+      <c r="AI2" t="str">
+        <v>Brand Satisfaction Level</v>
+      </c>
+      <c r="AJ2" t="str">
+        <v>Brand Fulfillment Capacity</v>
+      </c>
+      <c r="AK2" t="str">
+        <v>Design Importance Level</v>
+      </c>
+      <c r="AL2" t="str">
+        <v>Design Satisfaction Level</v>
+      </c>
+      <c r="AM2" t="str">
+        <v>Design Fulfillment Capacity</v>
+      </c>
+      <c r="AN2" t="str">
+        <v>Battery Importance Level</v>
+      </c>
+      <c r="AO2" t="str">
+        <v>Battery Satisfaction Level</v>
+      </c>
+      <c r="AP2" t="str">
+        <v>Battery Fulfillment Capacity</v>
+      </c>
+      <c r="AQ2" t="str">
+        <v>Weight Importance Level</v>
+      </c>
+      <c r="AR2" t="str">
+        <v>Weight Satisfaction Level</v>
+      </c>
+      <c r="AS2" t="str">
+        <v>Weight Fulfillment Capacity</v>
+      </c>
+      <c r="AT2" t="str">
+        <v>Safety Importance Level</v>
+      </c>
+      <c r="AU2" t="str">
+        <v>Safety Satisfaction Level</v>
+      </c>
+      <c r="AV2" t="str">
+        <v>Safety Fulfillment Capacity</v>
+      </c>
+      <c r="AW2" t="str">
+        <v>Price Importance Level</v>
+      </c>
+      <c r="AX2" t="str">
+        <v>Price Satisfaction Level</v>
+      </c>
+      <c r="AY2" t="str">
+        <v>Price Fulfillment Capacity</v>
+      </c>
+      <c r="AZ2" t="str">
+        <v>Maintenance Importance Level</v>
+      </c>
+      <c r="BA2" t="str">
+        <v>Maintenance Satisfaction Level</v>
+      </c>
+      <c r="BB2" t="str">
+        <v>Maintenance Fulfillment Capacity</v>
+      </c>
+      <c r="BC2" t="str">
+        <v>Social value Importance Level</v>
+      </c>
+      <c r="BD2" t="str">
+        <v>Social value Satisfaction Level</v>
+      </c>
+      <c r="BE2" t="str">
+        <v>Social value Fulfillment Capacity</v>
+      </c>
+      <c r="BF2" t="str">
+        <v>Re-sell value Importance Level</v>
+      </c>
+      <c r="BG2" t="str">
+        <v>Re-sell value Satisfaction Level</v>
+      </c>
+      <c r="BH2" t="str">
+        <v>Re-sell value Fulfillment Capacity</v>
+      </c>
+      <c r="BI2" t="str">
+        <v>Overall satisfaction Importance Level</v>
+      </c>
+      <c r="BJ2" t="str">
+        <v>Overall satisfaction Satisfaction Level</v>
+      </c>
+      <c r="BK2" t="str">
+        <v>Overall satisfaction Fulfillment Capacity</v>
+      </c>
+      <c r="BL2" t="str">
+        <v>Age</v>
+      </c>
+      <c r="BM2" t="str">
+        <v>Buy Vehicle in Future</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -663,61 +807,61 @@
         <v>01710151265</v>
       </c>
       <c r="C3" t="str">
-        <v>Sports</v>
+        <v>sports</v>
       </c>
       <c r="D3" t="str">
+        <v>4</v>
+      </c>
+      <c r="E3" t="str">
         <v>9</v>
       </c>
-      <c r="E3" t="str">
-        <v>5</v>
-      </c>
       <c r="F3" t="str">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
         <v>8</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
+        <v>10</v>
+      </c>
+      <c r="I3" t="str">
+        <v>14</v>
+      </c>
+      <c r="J3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K3" t="str">
+        <v>11</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2</v>
+      </c>
+      <c r="M3" t="str">
         <v>1</v>
       </c>
-      <c r="H3" t="str">
+      <c r="N3" t="str">
+        <v>12</v>
+      </c>
+      <c r="O3" t="str">
+        <v>7</v>
+      </c>
+      <c r="P3" t="str">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>5</v>
+      </c>
+      <c r="R3" t="str">
+        <v>13</v>
+      </c>
+      <c r="S3" t="str">
         <v>2</v>
       </c>
-      <c r="I3" t="str">
-        <v>3</v>
-      </c>
-      <c r="J3" t="str">
-        <v>13</v>
-      </c>
-      <c r="K3" t="str">
-        <v>12</v>
-      </c>
-      <c r="L3" t="str">
+      <c r="T3" t="str">
+        <v>6</v>
+      </c>
+      <c r="U3" t="str">
         <v>7</v>
-      </c>
-      <c r="M3" t="str">
-        <v>4</v>
-      </c>
-      <c r="N3" t="str">
-        <v>6</v>
-      </c>
-      <c r="O3" t="str">
-        <v>11</v>
-      </c>
-      <c r="P3" t="str">
-        <v>15</v>
-      </c>
-      <c r="Q3" t="str">
-        <v>14</v>
-      </c>
-      <c r="R3" t="str">
-        <v>10</v>
-      </c>
-      <c r="S3" t="str">
-        <v>3</v>
-      </c>
-      <c r="T3" t="str">
-        <v>5</v>
-      </c>
-      <c r="U3" t="str">
-        <v>5</v>
       </c>
       <c r="V3" t="str">
         <v>5</v>
@@ -729,28 +873,28 @@
         <v>5</v>
       </c>
       <c r="Y3" t="str">
+        <v>5</v>
+      </c>
+      <c r="Z3" t="str">
+        <v>6</v>
+      </c>
+      <c r="AA3" t="str">
         <v>4</v>
       </c>
-      <c r="Z3" t="str">
+      <c r="AB3" t="str">
+        <v>3</v>
+      </c>
+      <c r="AC3" t="str">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="str">
+        <v>5</v>
+      </c>
+      <c r="AE3" t="str">
         <v>2</v>
       </c>
-      <c r="AA3" t="str">
-        <v>5</v>
-      </c>
-      <c r="AB3" t="str">
-        <v>2</v>
-      </c>
-      <c r="AC3" t="str">
-        <v>5</v>
-      </c>
-      <c r="AD3" t="str">
-        <v>4</v>
-      </c>
-      <c r="AE3" t="str">
-        <v>6</v>
-      </c>
       <c r="AF3" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG3" t="str">
         <v>3</v>
@@ -759,28 +903,28 @@
         <v>5</v>
       </c>
       <c r="AI3" t="str">
+        <v>7</v>
+      </c>
+      <c r="AJ3" t="str">
+        <v>5</v>
+      </c>
+      <c r="AK3" t="str">
         <v>6</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AL3" t="str">
+        <v>6</v>
+      </c>
+      <c r="AM3" t="str">
         <v>2</v>
       </c>
-      <c r="AK3" t="str">
-        <v>3</v>
-      </c>
-      <c r="AL3" t="str">
-        <v>4</v>
-      </c>
-      <c r="AM3" t="str">
-        <v>5</v>
-      </c>
       <c r="AN3" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AO3" t="str">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AP3" t="str">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AQ3" t="str">
         <v>5</v>
@@ -795,65 +939,72 @@
         <v>4</v>
       </c>
       <c r="AU3" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AV3" t="str">
+        <v>1</v>
+      </c>
+      <c r="AW3" t="str">
         <v>4</v>
       </c>
-      <c r="AW3" t="str">
+      <c r="AX3" t="str">
+        <v>5</v>
+      </c>
+      <c r="AY3" t="str">
         <v>6</v>
       </c>
-      <c r="AX3" t="str">
+      <c r="AZ3" t="str">
         <v>6</v>
       </c>
-      <c r="AY3" t="str">
-        <v>3</v>
-      </c>
-      <c r="AZ3" t="str">
-        <v>2</v>
-      </c>
       <c r="BA3" t="str">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BB3" t="str">
         <v>4</v>
       </c>
       <c r="BC3" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD3" t="str">
         <v>4</v>
       </c>
       <c r="BE3" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF3" t="str">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="BG3" t="str">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="BH3" t="str">
         <v>5</v>
       </c>
       <c r="BI3" t="str">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BJ3" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BK3" t="str">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="BL3" t="str">
+        <v>26-35</v>
+      </c>
+      <c r="BM3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:R1"/>
     <mergeCell ref="S1:BK1"/>
+    <mergeCell ref="BL1:BM1"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BM3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BN3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>